<commit_message>
Diagramme auf 100% gestellt
</commit_message>
<xml_diff>
--- a/Validierung/coverage/ctm_3_coverage.xlsx
+++ b/Validierung/coverage/ctm_3_coverage.xlsx
@@ -851,11 +851,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="435868304"/>
-        <c:axId val="435870656"/>
+        <c:axId val="388309440"/>
+        <c:axId val="388304736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="435868304"/>
+        <c:axId val="388309440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -898,7 +898,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="435870656"/>
+        <c:crossAx val="388304736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -906,9 +906,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="435870656"/>
+        <c:axId val="388304736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -957,7 +958,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="435868304"/>
+        <c:crossAx val="388309440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>

</xml_diff>